<commit_message>
nâng cấp và cải thiện tính năng sản phẩm và giỏ hàng
</commit_message>
<xml_diff>
--- a/設計とテスト/エラーコード一覧.xlsx
+++ b/設計とテスト/エラーコード一覧.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>コード</t>
     <phoneticPr fontId="1"/>
@@ -206,6 +206,54 @@
   </si>
   <si>
     <t>lỗi liên quan đến các loại token</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0008</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lỗi liên quan đến sản phẩm</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0009</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>định dạng hình ảnh không đúng</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0008</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Định dạng hình ảnh không chính xác</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lưu hình ảnh thất bại</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0009</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{0} thất bại</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -556,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -641,6 +689,30 @@
         <v>38</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -653,7 +725,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -809,15 +881,33 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>MSG_W0008</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>MSG_W0009</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>